<commit_message>
Fin avec test des utilisateurs connectés avec javadoc et xcel temps
</commit_message>
<xml_diff>
--- a/Fonctionnalites a developper.xlsx
+++ b/Fonctionnalites a developper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myoffice.accenture.com/personal/marion_lucas_accenture_com/Documents/Bureau/Cours/Projet/projet-concession/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{7BA4A5E9-57A1-334E-88B0-8185AA947058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C0C05B2-378E-4BA1-8FDA-780EEBD22CEF}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{7BA4A5E9-57A1-334E-88B0-8185AA947058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D9628D6-4367-4A14-AD10-0815144EDDE4}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CC5C8F08-0244-0748-9807-3B43C892A48C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="128">
   <si>
     <t>APPLICATION DE LOCATION DE VEHICULES</t>
   </si>
@@ -414,6 +414,12 @@
   </si>
   <si>
     <t>1h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">problèmes avec les tests et oublie qu'il fallait le faire sur Client et User donc plus de temps pris </t>
+  </si>
+  <si>
+    <t>4h</t>
   </si>
 </sst>
 </file>
@@ -511,6 +517,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -810,10 +820,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30024EB3-F791-9945-8DAE-0E5226717322}">
-  <dimension ref="A1:I135"/>
+  <dimension ref="A1:J135"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -826,9 +836,10 @@
     <col min="6" max="7" width="15.8984375" customWidth="1"/>
     <col min="8" max="8" width="92" customWidth="1"/>
     <col min="9" max="9" width="70.8984375" customWidth="1"/>
+    <col min="10" max="10" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="54.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="54.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -841,7 +852,7 @@
       <c r="H1" s="7"/>
       <c r="I1" s="7"/>
     </row>
-    <row r="2" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
@@ -854,7 +865,7 @@
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
     </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -883,7 +894,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="41.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="41.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -910,7 +921,7 @@
       </c>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9" ht="41.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="41.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -939,7 +950,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="57.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="57.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -968,7 +979,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -997,7 +1008,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -1017,7 +1028,7 @@
         <v>124</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>29</v>
@@ -1025,8 +1036,11 @@
       <c r="I8" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="J8" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -1051,7 +1065,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -1076,7 +1090,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>1</v>
       </c>
@@ -1101,7 +1115,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>1</v>
       </c>
@@ -1126,7 +1140,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>1</v>
       </c>
@@ -1151,7 +1165,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>1</v>
       </c>
@@ -1176,7 +1190,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>1</v>
       </c>
@@ -1201,7 +1215,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>2</v>
       </c>
@@ -2664,6 +2678,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="8824ee56-782f-421a-8485-dc2b27327db7" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00dc33ae-35e0-45d6-a075-19848b495adf">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008222304C56FCA048A7A2CE156CED619F" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3027a3f7c6c7c5e5241019623fec96f5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00dc33ae-35e0-45d6-a075-19848b495adf" xmlns:ns3="8824ee56-782f-421a-8485-dc2b27327db7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="70240a01ac339efc7b557cad56c25de9" ns2:_="" ns3:_="">
     <xsd:import namespace="00dc33ae-35e0-45d6-a075-19848b495adf"/>
@@ -2858,27 +2892,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5A04AB8-1287-43C7-A7AC-07423B257B0D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="8824ee56-782f-421a-8485-dc2b27327db7"/>
+    <ds:schemaRef ds:uri="00dc33ae-35e0-45d6-a075-19848b495adf"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="8824ee56-782f-421a-8485-dc2b27327db7" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00dc33ae-35e0-45d6-a075-19848b495adf">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDB49F5A-C68D-427D-B380-1B6A8E424C11}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B6E18EE-B9BA-4643-B0B7-0946341F48CA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2895,23 +2928,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDB49F5A-C68D-427D-B380-1B6A8E424C11}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5A04AB8-1287-43C7-A7AC-07423B257B0D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="8824ee56-782f-421a-8485-dc2b27327db7"/>
-    <ds:schemaRef ds:uri="00dc33ae-35e0-45d6-a075-19848b495adf"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fin de journée. RIP MARION
</commit_message>
<xml_diff>
--- a/Fonctionnalites a developper.xlsx
+++ b/Fonctionnalites a developper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myoffice.accenture.com/personal/marion_lucas_accenture_com/Documents/Bureau/Cours/Projet/projet-concession/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{7BA4A5E9-57A1-334E-88B0-8185AA947058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D9628D6-4367-4A14-AD10-0815144EDDE4}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{7BA4A5E9-57A1-334E-88B0-8185AA947058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DCC704B1-DD55-4DFE-ADF0-4500F96CDE5C}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CC5C8F08-0244-0748-9807-3B43C892A48C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="129">
   <si>
     <t>APPLICATION DE LOCATION DE VEHICULES</t>
   </si>
@@ -420,6 +420,9 @@
   </si>
   <si>
     <t>4h</t>
+  </si>
+  <si>
+    <t>2h (début 15h30)</t>
   </si>
 </sst>
 </file>
@@ -822,8 +825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30024EB3-F791-9945-8DAE-0E5226717322}">
   <dimension ref="A1:J135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="C3" zoomScale="84" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1056,7 +1059,9 @@
       <c r="E9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="1"/>
+      <c r="F9" s="1" t="s">
+        <v>128</v>
+      </c>
       <c r="G9" s="1"/>
       <c r="H9" s="3" t="s">
         <v>34</v>
@@ -2689,15 +2694,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008222304C56FCA048A7A2CE156CED619F" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3027a3f7c6c7c5e5241019623fec96f5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00dc33ae-35e0-45d6-a075-19848b495adf" xmlns:ns3="8824ee56-782f-421a-8485-dc2b27327db7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="70240a01ac339efc7b557cad56c25de9" ns2:_="" ns3:_="">
     <xsd:import namespace="00dc33ae-35e0-45d6-a075-19848b495adf"/>
@@ -2892,6 +2888,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5A04AB8-1287-43C7-A7AC-07423B257B0D}">
   <ds:schemaRefs>
@@ -2904,14 +2909,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDB49F5A-C68D-427D-B380-1B6A8E424C11}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B6E18EE-B9BA-4643-B0B7-0946341F48CA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2928,4 +2925,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDB49F5A-C68D-427D-B380-1B6A8E424C11}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Normalement les Utilisateurs sont vraiment fini
</commit_message>
<xml_diff>
--- a/Fonctionnalites a developper.xlsx
+++ b/Fonctionnalites a developper.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myoffice.accenture.com/personal/marion_lucas_accenture_com/Documents/Bureau/Cours/Projet/projet-concession/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{7BA4A5E9-57A1-334E-88B0-8185AA947058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DCC704B1-DD55-4DFE-ADF0-4500F96CDE5C}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="13_ncr:1_{7BA4A5E9-57A1-334E-88B0-8185AA947058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D3CA0DBA-4672-4618-A77A-26F44954DD22}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CC5C8F08-0244-0748-9807-3B43C892A48C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CC5C8F08-0244-0748-9807-3B43C892A48C}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="135">
   <si>
     <t>APPLICATION DE LOCATION DE VEHICULES</t>
   </si>
@@ -423,6 +423,24 @@
   </si>
   <si>
     <t>2h (début 15h30)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pour création des différentes classes concernant Véhicules et voiture, ainsi que la réalisation des tests / Fait en même temps que l'affichage du par cet de la voiture particulière </t>
+  </si>
+  <si>
+    <t>CF Ajout voiture car tout fait en même temps</t>
+  </si>
+  <si>
+    <t>1h30</t>
+  </si>
+  <si>
+    <t>3h au moins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plusieurs soucis ce sont présentés, Emmanuel n'étais pas dispo et j'ai du patienté. Puis les tests ne fonctionnaient pas comme voulu.Couverture pas à 100% je pense qu'il faudra les revoir au moment des tests plus tard. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3h (début 15h40) </t>
   </si>
 </sst>
 </file>
@@ -520,10 +538,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -825,8 +839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30024EB3-F791-9945-8DAE-0E5226717322}">
   <dimension ref="A1:J135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C3" zoomScale="84" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -836,10 +850,11 @@
     <col min="3" max="3" width="30.59765625" customWidth="1"/>
     <col min="4" max="4" width="14.09765625" style="6" customWidth="1"/>
     <col min="5" max="5" width="46.09765625" customWidth="1"/>
-    <col min="6" max="7" width="15.8984375" customWidth="1"/>
+    <col min="6" max="6" width="38.19921875" customWidth="1"/>
+    <col min="7" max="7" width="15.8984375" customWidth="1"/>
     <col min="8" max="8" width="92" customWidth="1"/>
     <col min="9" max="9" width="70.8984375" customWidth="1"/>
-    <col min="10" max="10" width="11" customWidth="1"/>
+    <col min="10" max="10" width="110.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="54.9" customHeight="1" x14ac:dyDescent="0.3">
@@ -1062,12 +1077,17 @@
       <c r="F9" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="G9" s="1"/>
+      <c r="G9" s="1" t="s">
+        <v>127</v>
+      </c>
       <c r="H9" s="3" t="s">
         <v>34</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>18</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
@@ -1086,7 +1106,9 @@
       <c r="E10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F10" s="1"/>
+      <c r="F10" s="1" t="s">
+        <v>130</v>
+      </c>
       <c r="G10" s="1"/>
       <c r="H10" s="3" t="s">
         <v>37</v>
@@ -1111,7 +1133,9 @@
       <c r="E11" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F11" s="1"/>
+      <c r="F11" s="1" t="s">
+        <v>130</v>
+      </c>
       <c r="G11" s="1"/>
       <c r="H11" s="3" t="s">
         <v>40</v>
@@ -1136,13 +1160,20 @@
       <c r="E12" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
+      <c r="F12" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>132</v>
+      </c>
       <c r="H12" s="3" t="s">
         <v>43</v>
       </c>
       <c r="I12" s="3" t="s">
         <v>18</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
@@ -1161,7 +1192,9 @@
       <c r="E13" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F13" s="1"/>
+      <c r="F13" s="1" t="s">
+        <v>134</v>
+      </c>
       <c r="G13" s="1"/>
       <c r="H13" s="3" t="s">
         <v>46</v>
@@ -2694,6 +2727,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008222304C56FCA048A7A2CE156CED619F" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3027a3f7c6c7c5e5241019623fec96f5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00dc33ae-35e0-45d6-a075-19848b495adf" xmlns:ns3="8824ee56-782f-421a-8485-dc2b27327db7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="70240a01ac339efc7b557cad56c25de9" ns2:_="" ns3:_="">
     <xsd:import namespace="00dc33ae-35e0-45d6-a075-19848b495adf"/>
@@ -2888,15 +2930,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5A04AB8-1287-43C7-A7AC-07423B257B0D}">
   <ds:schemaRefs>
@@ -2909,6 +2942,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDB49F5A-C68D-427D-B380-1B6A8E424C11}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B6E18EE-B9BA-4643-B0B7-0946341F48CA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2925,12 +2966,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDB49F5A-C68D-427D-B380-1B6A8E424C11}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fin de la gestion des véhicules
</commit_message>
<xml_diff>
--- a/Fonctionnalites a developper.xlsx
+++ b/Fonctionnalites a developper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myoffice.accenture.com/personal/marion_lucas_accenture_com/Documents/Bureau/Cours/Projet/projet-concession/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="13_ncr:1_{7BA4A5E9-57A1-334E-88B0-8185AA947058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D3CA0DBA-4672-4618-A77A-26F44954DD22}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="13_ncr:1_{7BA4A5E9-57A1-334E-88B0-8185AA947058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8E719BE-78DC-47B0-94AB-9BA260FA36BC}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CC5C8F08-0244-0748-9807-3B43C892A48C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="140">
   <si>
     <t>APPLICATION DE LOCATION DE VEHICULES</t>
   </si>
@@ -441,6 +441,21 @@
   </si>
   <si>
     <t xml:space="preserve">3h (début 15h40) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1J </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calcul temps très mal fait car beaucoup de choses à revoir avant de pouvoir finir totalement ce que j'avais fais. Notamment dans client/ admin / les filtres, etc </t>
+  </si>
+  <si>
+    <t>1journée</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3h (car pas fait de velo, juste moto) </t>
+  </si>
+  <si>
+    <t>3h (début 14h00)</t>
   </si>
 </sst>
 </file>
@@ -839,8 +854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30024EB3-F791-9945-8DAE-0E5226717322}">
   <dimension ref="A1:J135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -850,8 +865,8 @@
     <col min="3" max="3" width="30.59765625" customWidth="1"/>
     <col min="4" max="4" width="14.09765625" style="6" customWidth="1"/>
     <col min="5" max="5" width="46.09765625" customWidth="1"/>
-    <col min="6" max="6" width="38.19921875" customWidth="1"/>
-    <col min="7" max="7" width="15.8984375" customWidth="1"/>
+    <col min="6" max="6" width="49.09765625" customWidth="1"/>
+    <col min="7" max="7" width="35.5" customWidth="1"/>
     <col min="8" max="8" width="92" customWidth="1"/>
     <col min="9" max="9" width="70.8984375" customWidth="1"/>
     <col min="10" max="10" width="110.5" customWidth="1"/>
@@ -1195,12 +1210,17 @@
       <c r="F13" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="G13" s="1"/>
+      <c r="G13" s="1" t="s">
+        <v>135</v>
+      </c>
       <c r="H13" s="3" t="s">
         <v>46</v>
       </c>
       <c r="I13" s="3" t="s">
         <v>18</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
@@ -1219,8 +1239,12 @@
       <c r="E14" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
+      <c r="F14" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>138</v>
+      </c>
       <c r="H14" s="3" t="s">
         <v>49</v>
       </c>
@@ -1244,7 +1268,9 @@
       <c r="E15" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F15" s="1"/>
+      <c r="F15" s="1" t="s">
+        <v>139</v>
+      </c>
       <c r="G15" s="1"/>
       <c r="H15" s="3" t="s">
         <v>52</v>
@@ -2716,26 +2742,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="8824ee56-782f-421a-8485-dc2b27327db7" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00dc33ae-35e0-45d6-a075-19848b495adf">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008222304C56FCA048A7A2CE156CED619F" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3027a3f7c6c7c5e5241019623fec96f5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00dc33ae-35e0-45d6-a075-19848b495adf" xmlns:ns3="8824ee56-782f-421a-8485-dc2b27327db7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="70240a01ac339efc7b557cad56c25de9" ns2:_="" ns3:_="">
     <xsd:import namespace="00dc33ae-35e0-45d6-a075-19848b495adf"/>
@@ -2930,26 +2936,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5A04AB8-1287-43C7-A7AC-07423B257B0D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="8824ee56-782f-421a-8485-dc2b27327db7"/>
-    <ds:schemaRef ds:uri="00dc33ae-35e0-45d6-a075-19848b495adf"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="8824ee56-782f-421a-8485-dc2b27327db7" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00dc33ae-35e0-45d6-a075-19848b495adf">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDB49F5A-C68D-427D-B380-1B6A8E424C11}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B6E18EE-B9BA-4643-B0B7-0946341F48CA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2966,4 +2973,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5A04AB8-1287-43C7-A7AC-07423B257B0D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="8824ee56-782f-421a-8485-dc2b27327db7"/>
+    <ds:schemaRef ds:uri="00dc33ae-35e0-45d6-a075-19848b495adf"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDB49F5A-C68D-427D-B380-1B6A8E424C11}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Swagger sans log + Recherche par dates + Parc afficher complet
</commit_message>
<xml_diff>
--- a/Fonctionnalites a developper.xlsx
+++ b/Fonctionnalites a developper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myoffice.accenture.com/personal/marion_lucas_accenture_com/Documents/Bureau/Cours/Projet/projet-concession/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="13_ncr:1_{7BA4A5E9-57A1-334E-88B0-8185AA947058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8E719BE-78DC-47B0-94AB-9BA260FA36BC}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="13_ncr:1_{7BA4A5E9-57A1-334E-88B0-8185AA947058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA177D40-05FF-44D7-BA78-8CACE79AE568}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CC5C8F08-0244-0748-9807-3B43C892A48C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="141">
   <si>
     <t>APPLICATION DE LOCATION DE VEHICULES</t>
   </si>
@@ -456,6 +456,9 @@
   </si>
   <si>
     <t>3h (début 14h00)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4h30 </t>
   </si>
 </sst>
 </file>
@@ -555,8 +558,12 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
@@ -855,10 +862,10 @@
   <dimension ref="A1:J135"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.09765625" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
@@ -1271,7 +1278,9 @@
       <c r="F15" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="G15" s="1"/>
+      <c r="G15" s="1" t="s">
+        <v>140</v>
+      </c>
       <c r="H15" s="3" t="s">
         <v>52</v>
       </c>
@@ -1295,8 +1304,12 @@
       <c r="E16" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
+      <c r="F16" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>127</v>
+      </c>
       <c r="H16" s="3" t="s">
         <v>56</v>
       </c>
@@ -2742,6 +2755,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="8824ee56-782f-421a-8485-dc2b27327db7" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00dc33ae-35e0-45d6-a075-19848b495adf">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008222304C56FCA048A7A2CE156CED619F" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3027a3f7c6c7c5e5241019623fec96f5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00dc33ae-35e0-45d6-a075-19848b495adf" xmlns:ns3="8824ee56-782f-421a-8485-dc2b27327db7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="70240a01ac339efc7b557cad56c25de9" ns2:_="" ns3:_="">
     <xsd:import namespace="00dc33ae-35e0-45d6-a075-19848b495adf"/>
@@ -2936,27 +2969,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="8824ee56-782f-421a-8485-dc2b27327db7" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00dc33ae-35e0-45d6-a075-19848b495adf">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDB49F5A-C68D-427D-B380-1B6A8E424C11}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5A04AB8-1287-43C7-A7AC-07423B257B0D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="8824ee56-782f-421a-8485-dc2b27327db7"/>
+    <ds:schemaRef ds:uri="00dc33ae-35e0-45d6-a075-19848b495adf"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B6E18EE-B9BA-4643-B0B7-0946341F48CA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2973,23 +3005,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5A04AB8-1287-43C7-A7AC-07423B257B0D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="8824ee56-782f-421a-8485-dc2b27327db7"/>
-    <ds:schemaRef ds:uri="00dc33ae-35e0-45d6-a075-19848b495adf"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDB49F5A-C68D-427D-B380-1B6A8E424C11}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Rechercher par date & rechercher par dates/catégories
</commit_message>
<xml_diff>
--- a/Fonctionnalites a developper.xlsx
+++ b/Fonctionnalites a developper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myoffice.accenture.com/personal/marion_lucas_accenture_com/Documents/Bureau/Cours/Projet/projet-concession/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="54" documentId="13_ncr:1_{7BA4A5E9-57A1-334E-88B0-8185AA947058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA177D40-05FF-44D7-BA78-8CACE79AE568}"/>
+  <xr:revisionPtr revIDLastSave="55" documentId="13_ncr:1_{7BA4A5E9-57A1-334E-88B0-8185AA947058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A416E21-A230-4B10-B966-AE8616146E0C}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CC5C8F08-0244-0748-9807-3B43C892A48C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="142">
   <si>
     <t>APPLICATION DE LOCATION DE VEHICULES</t>
   </si>
@@ -459,6 +459,9 @@
   </si>
   <si>
     <t xml:space="preserve">4h30 </t>
+  </si>
+  <si>
+    <t>3h (début 10h30)</t>
   </si>
 </sst>
 </file>
@@ -1333,7 +1336,9 @@
       <c r="E17" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F17" s="1"/>
+      <c r="F17" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="G17" s="1"/>
       <c r="H17" s="3" t="s">
         <v>60</v>
@@ -2764,17 +2769,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="8824ee56-782f-421a-8485-dc2b27327db7" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00dc33ae-35e0-45d6-a075-19848b495adf">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008222304C56FCA048A7A2CE156CED619F" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3027a3f7c6c7c5e5241019623fec96f5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00dc33ae-35e0-45d6-a075-19848b495adf" xmlns:ns3="8824ee56-782f-421a-8485-dc2b27327db7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="70240a01ac339efc7b557cad56c25de9" ns2:_="" ns3:_="">
     <xsd:import namespace="00dc33ae-35e0-45d6-a075-19848b495adf"/>
@@ -2969,6 +2963,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="8824ee56-782f-421a-8485-dc2b27327db7" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00dc33ae-35e0-45d6-a075-19848b495adf">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDB49F5A-C68D-427D-B380-1B6A8E424C11}">
   <ds:schemaRefs>
@@ -2978,17 +2983,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5A04AB8-1287-43C7-A7AC-07423B257B0D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="8824ee56-782f-421a-8485-dc2b27327db7"/>
-    <ds:schemaRef ds:uri="00dc33ae-35e0-45d6-a075-19848b495adf"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B6E18EE-B9BA-4643-B0B7-0946341F48CA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3005,4 +2999,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5A04AB8-1287-43C7-A7AC-07423B257B0D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="8824ee56-782f-421a-8485-dc2b27327db7"/>
+    <ds:schemaRef ds:uri="00dc33ae-35e0-45d6-a075-19848b495adf"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Projet Dernières modifs avant présentations
</commit_message>
<xml_diff>
--- a/Fonctionnalites a developper.xlsx
+++ b/Fonctionnalites a developper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myoffice.accenture.com/personal/marion_lucas_accenture_com/Documents/Bureau/Cours/Projet/projet-concession/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="55" documentId="13_ncr:1_{7BA4A5E9-57A1-334E-88B0-8185AA947058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A416E21-A230-4B10-B966-AE8616146E0C}"/>
+  <xr:revisionPtr revIDLastSave="60" documentId="13_ncr:1_{7BA4A5E9-57A1-334E-88B0-8185AA947058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2078F85A-239F-48C0-B02C-BA5AFC4230DA}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CC5C8F08-0244-0748-9807-3B43C892A48C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="144">
   <si>
     <t>APPLICATION DE LOCATION DE VEHICULES</t>
   </si>
@@ -462,6 +462,12 @@
   </si>
   <si>
     <t>3h (début 10h30)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3h en regroupant toutes les recherches </t>
+  </si>
+  <si>
+    <t>'</t>
   </si>
 </sst>
 </file>
@@ -523,7 +529,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -544,6 +550,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -559,10 +568,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -865,7 +870,7 @@
   <dimension ref="A1:J135"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1339,7 +1344,9 @@
       <c r="F17" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="G17" s="1"/>
+      <c r="G17" s="1" t="s">
+        <v>142</v>
+      </c>
       <c r="H17" s="3" t="s">
         <v>60</v>
       </c>
@@ -1363,8 +1370,12 @@
       <c r="E18" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
+      <c r="F18" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>143</v>
+      </c>
       <c r="H18" s="3" t="s">
         <v>63</v>
       </c>
@@ -1388,8 +1399,12 @@
       <c r="E19" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
+      <c r="F19" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>143</v>
+      </c>
       <c r="H19" s="3" t="s">
         <v>67</v>
       </c>
@@ -2769,6 +2784,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="8824ee56-782f-421a-8485-dc2b27327db7" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00dc33ae-35e0-45d6-a075-19848b495adf">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008222304C56FCA048A7A2CE156CED619F" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3027a3f7c6c7c5e5241019623fec96f5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00dc33ae-35e0-45d6-a075-19848b495adf" xmlns:ns3="8824ee56-782f-421a-8485-dc2b27327db7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="70240a01ac339efc7b557cad56c25de9" ns2:_="" ns3:_="">
     <xsd:import namespace="00dc33ae-35e0-45d6-a075-19848b495adf"/>
@@ -2963,17 +2989,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="8824ee56-782f-421a-8485-dc2b27327db7" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00dc33ae-35e0-45d6-a075-19848b495adf">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDB49F5A-C68D-427D-B380-1B6A8E424C11}">
   <ds:schemaRefs>
@@ -2983,6 +2998,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5A04AB8-1287-43C7-A7AC-07423B257B0D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="8824ee56-782f-421a-8485-dc2b27327db7"/>
+    <ds:schemaRef ds:uri="00dc33ae-35e0-45d6-a075-19848b495adf"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B6E18EE-B9BA-4643-B0B7-0946341F48CA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2999,15 +3025,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5A04AB8-1287-43C7-A7AC-07423B257B0D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="8824ee56-782f-421a-8485-dc2b27327db7"/>
-    <ds:schemaRef ds:uri="00dc33ae-35e0-45d6-a075-19848b495adf"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>